<commit_message>
Completed with new updates
</commit_message>
<xml_diff>
--- a/sku.xlsx
+++ b/sku.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\scrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E782352F-1D24-42D9-A2A7-0E7D48F5CFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257A023B-5E84-4AF2-AD31-6163D4219609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>SKU</t>
   </si>
   <si>
-    <t>UNV61683</t>
-  </si>
-  <si>
-    <t>AVE17575</t>
-  </si>
-  <si>
-    <t>E5148120</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>A5597500MG</t>
-  </si>
-  <si>
-    <t>K55115US</t>
-  </si>
-  <si>
-    <t>K97206US</t>
+    <t>AMR1042183</t>
+  </si>
+  <si>
+    <t>AMR1033676</t>
+  </si>
+  <si>
+    <t>AMRRL72845</t>
+  </si>
+  <si>
+    <t>AMR1003094</t>
+  </si>
+  <si>
+    <t>AMR1003261</t>
+  </si>
+  <si>
+    <t>AMR1001620</t>
+  </si>
+  <si>
+    <t>AMR1003121</t>
+  </si>
+  <si>
+    <t>AMR1003110</t>
+  </si>
+  <si>
+    <t>AMR1003020</t>
+  </si>
+  <si>
+    <t>ZPE1041414</t>
+  </si>
+  <si>
+    <t>ZEB75005</t>
+  </si>
+  <si>
+    <t>ZEB75050</t>
+  </si>
+  <si>
+    <t>ZEB45511</t>
+  </si>
+  <si>
+    <t>ZEB10613</t>
+  </si>
+  <si>
+    <t>ZEB87012</t>
+  </si>
+  <si>
+    <t>ZEB87032</t>
+  </si>
+  <si>
+    <t>ZEB78105</t>
+  </si>
+  <si>
+    <t>ZEB88112</t>
+  </si>
+  <si>
+    <t>ZEB88122</t>
   </si>
 </sst>
 </file>
@@ -113,7 +149,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -126,6 +161,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,235 +445,275 @@
   <dimension ref="A1:A134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="27" style="3" customWidth="1"/>
+    <col min="1" max="1" width="27" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
-        <v>65590</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="7" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="8" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="14" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-    </row>
-    <row r="18" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-    </row>
-    <row r="23" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
-    </row>
-    <row r="24" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-    </row>
-    <row r="27" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
-    </row>
-    <row r="28" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A28" s="5"/>
+    <row r="9" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A28" s="4"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A31" s="4"/>
+      <c r="A31" s="3"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A32" s="5"/>
+      <c r="A32" s="4"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A35" s="4"/>
+      <c r="A35" s="3"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A36" s="5"/>
+      <c r="A36" s="4"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A39" s="4"/>
+      <c r="A39" s="3"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A40" s="5"/>
+      <c r="A40" s="4"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A43" s="4"/>
+      <c r="A43" s="3"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A44" s="5"/>
+      <c r="A44" s="4"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A47" s="4"/>
+      <c r="A47" s="3"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A48" s="5"/>
+      <c r="A48" s="4"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A51" s="4"/>
+      <c r="A51" s="3"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A52" s="5"/>
+      <c r="A52" s="4"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A55" s="4"/>
+      <c r="A55" s="3"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A56" s="5"/>
+      <c r="A56" s="4"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A59" s="4"/>
+      <c r="A59" s="3"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A60" s="5"/>
+      <c r="A60" s="4"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A63" s="4"/>
+      <c r="A63" s="3"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A64" s="5"/>
+      <c r="A64" s="4"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A67" s="4"/>
+      <c r="A67" s="3"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A68" s="5"/>
+      <c r="A68" s="4"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A71" s="4"/>
+      <c r="A71" s="3"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A72" s="5"/>
+      <c r="A72" s="4"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A75" s="4"/>
+      <c r="A75" s="3"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A76" s="5"/>
+      <c r="A76" s="4"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A79" s="4"/>
+      <c r="A79" s="3"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A80" s="5"/>
+      <c r="A80" s="4"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A83" s="4"/>
+      <c r="A83" s="3"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A84" s="5"/>
+      <c r="A84" s="4"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A87" s="4"/>
+      <c r="A87" s="3"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A88" s="5"/>
+      <c r="A88" s="4"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A91" s="4"/>
+      <c r="A91" s="3"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A92" s="5"/>
+      <c r="A92" s="4"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A95" s="4"/>
+      <c r="A95" s="3"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A96" s="5"/>
+      <c r="A96" s="4"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A99" s="4"/>
+      <c r="A99" s="3"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A100" s="5"/>
+      <c r="A100" s="4"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A103" s="4"/>
+      <c r="A103" s="3"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A104" s="5"/>
+      <c r="A104" s="4"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A108" s="4"/>
+      <c r="A108" s="3"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A109" s="5"/>
+      <c r="A109" s="4"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A113" s="4"/>
+      <c r="A113" s="3"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A114" s="5"/>
+      <c r="A114" s="4"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A118" s="4"/>
+      <c r="A118" s="3"/>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A119" s="5"/>
+      <c r="A119" s="4"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A123" s="4"/>
+      <c r="A123" s="3"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A124" s="5"/>
+      <c r="A124" s="4"/>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A128" s="4"/>
+      <c r="A128" s="3"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A129" s="5"/>
+      <c r="A129" s="4"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A133" s="4"/>
+      <c r="A133" s="3"/>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A134" s="5"/>
+      <c r="A134" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>